<commit_message>
adding sprites and game refactor
</commit_message>
<xml_diff>
--- a/dist/data/basetypes.xlsx
+++ b/dist/data/basetypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\Website\call-to-vocation\dist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DB712C-4C29-4DBC-BB3A-E0206D9425A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4741FA-E2F4-4DAE-A826-1182C1D36327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5370" windowWidth="29040" windowHeight="15840" xr2:uid="{82DCC3D5-4836-4E9E-8A18-9BC2420AB39E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{82DCC3D5-4836-4E9E-8A18-9BC2420AB39E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Scrap</t>
   </si>
   <si>
-    <t>Hoe</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>{"modName":"itemPower","modValue":15}</t>
+  </si>
+  <si>
+    <t>Spade</t>
   </si>
 </sst>
 </file>
@@ -496,12 +496,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1ED0B5F-E042-48D5-ACFB-41F9FE3E42B6}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -541,25 +543,25 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -567,25 +569,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -593,25 +595,25 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -619,25 +621,25 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -645,25 +647,25 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -671,25 +673,25 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -697,25 +699,25 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -723,25 +725,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -749,48 +751,48 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -798,25 +800,25 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -824,25 +826,25 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14">
         <v>5</v>
@@ -850,25 +852,25 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15">
         <v>5</v>
@@ -876,25 +878,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16">
         <v>5</v>
@@ -902,25 +904,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H17">
         <v>5</v>
@@ -928,25 +930,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -954,25 +956,25 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H19">
         <v>5</v>
@@ -980,25 +982,25 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H20">
         <v>5</v>
@@ -1006,25 +1008,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H21">
         <v>20</v>
@@ -1032,25 +1034,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H22">
         <v>20</v>
@@ -1058,25 +1060,25 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H23">
         <v>20</v>
@@ -1084,25 +1086,25 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H24">
         <v>20</v>
@@ -1110,25 +1112,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H25">
         <v>20</v>
@@ -1136,25 +1138,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H26">
         <v>20</v>
@@ -1162,25 +1164,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H27">
         <v>20</v>
@@ -1188,25 +1190,25 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H28">
         <v>20</v>
@@ -1214,25 +1216,25 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H29">
         <v>20</v>
@@ -1240,25 +1242,25 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H30">
         <v>100</v>
@@ -1266,25 +1268,25 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H31">
         <v>100</v>
@@ -1292,25 +1294,25 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H32">
         <v>100</v>
@@ -1318,25 +1320,25 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H33">
         <v>100</v>
@@ -1344,25 +1346,25 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H34">
         <v>100</v>
@@ -1370,25 +1372,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H35">
         <v>100</v>
@@ -1396,25 +1398,25 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H36">
         <v>100</v>
@@ -1422,25 +1424,25 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H37">
         <v>100</v>
@@ -1448,25 +1450,25 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H38">
         <v>100</v>
@@ -1474,25 +1476,25 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H39">
         <v>1000</v>
@@ -1500,25 +1502,25 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H40">
         <v>1000</v>
@@ -1526,25 +1528,25 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H41">
         <v>1000</v>
@@ -1552,25 +1554,25 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H42">
         <v>1000</v>
@@ -1578,25 +1580,25 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E43" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H43">
         <v>1000</v>
@@ -1604,25 +1606,25 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H44">
         <v>1000</v>
@@ -1630,25 +1632,25 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H45">
         <v>1000</v>
@@ -1656,25 +1658,25 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H46">
         <v>1000</v>
@@ -1682,25 +1684,25 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H47">
         <v>1000</v>

</xml_diff>

<commit_message>
redo game logic and tool upgrading
</commit_message>
<xml_diff>
--- a/dist/data/basetypes.xlsx
+++ b/dist/data/basetypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\Website\vocation-reroll\dist\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B27058-3F7C-4BD3-9D08-B3023E3312C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F735A42-8EB6-4EEE-984B-A2261D0B48A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22365" yWindow="8670" windowWidth="18000" windowHeight="9480" xr2:uid="{82DCC3D5-4836-4E9E-8A18-9BC2420AB39E}"/>
+    <workbookView xWindow="-28920" yWindow="5370" windowWidth="29040" windowHeight="15840" xr2:uid="{82DCC3D5-4836-4E9E-8A18-9BC2420AB39E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="44">
   <si>
     <t>name : String</t>
   </si>
@@ -132,22 +132,31 @@
     <t>resources : Array</t>
   </si>
   <si>
-    <t>{"resourceType":"wood","amount":5}</t>
-  </si>
-  <si>
     <t>Wooden</t>
   </si>
   <si>
-    <t>{"resourceType":"wood","amount":5}, {"resourceType":"copper","amount":5}</t>
-  </si>
-  <si>
-    <t>{"resourceType":"wood","amount":5}, {"resourceType":"silver","amount":5}</t>
-  </si>
-  <si>
-    <t>{"resourceType":"wood","amount":5}, {"resourceType":"gold","amount":5}</t>
-  </si>
-  <si>
-    <t>Golden</t>
+    <t>{"resourceType":"wood","amount":100}</t>
+  </si>
+  <si>
+    <t>{"resourceType":"wood","amount":100}, {"resourceType":"copper","amount":100}</t>
+  </si>
+  <si>
+    <t>{"modName":"itemPower","modValue":7}</t>
+  </si>
+  <si>
+    <t>{"resourceType":"wood","amount":100}, {"resourceType":"silver","amount":100}</t>
+  </si>
+  <si>
+    <t>{"resourceType":"wood","amount":100}, {"resourceType":"gold","amount":100}</t>
+  </si>
+  <si>
+    <t>Scales</t>
+  </si>
+  <si>
+    <t>Holy Symbol</t>
+  </si>
+  <si>
+    <t>Gold</t>
   </si>
 </sst>
 </file>
@@ -500,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1ED0B5F-E042-48D5-ACFB-41F9FE3E42B6}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +564,7 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -707,59 +716,55 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -767,16 +772,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>5</v>
@@ -787,16 +792,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>5</v>
@@ -807,16 +812,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>5</v>
@@ -827,16 +832,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -847,16 +852,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>5</v>
@@ -867,16 +872,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>5</v>
@@ -887,82 +892,82 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F22">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F23">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F24">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,7 +975,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
@@ -979,7 +984,7 @@
         <v>37</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F25">
         <v>20</v>
@@ -990,7 +995,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>25</v>
@@ -1010,7 +1015,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>25</v>
@@ -1030,7 +1035,7 @@
         <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>25</v>
@@ -1050,7 +1055,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>25</v>
@@ -1067,122 +1072,122 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F30">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F31">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F32">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F33">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F34">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F35">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1190,16 +1195,16 @@
         <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F36">
         <v>100</v>
@@ -1210,13 +1215,13 @@
         <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>20</v>
@@ -1230,13 +1235,13 @@
         <v>15</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>20</v>
@@ -1247,10 +1252,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>25</v>
@@ -1259,18 +1264,18 @@
         <v>39</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F39">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>25</v>
@@ -1279,18 +1284,18 @@
         <v>39</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F40">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>25</v>
@@ -1299,18 +1304,18 @@
         <v>39</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F41">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>25</v>
@@ -1319,18 +1324,18 @@
         <v>39</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F42">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>25</v>
@@ -1339,18 +1344,18 @@
         <v>39</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F43">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>25</v>
@@ -1359,18 +1364,18 @@
         <v>39</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F44">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>25</v>
@@ -1379,18 +1384,18 @@
         <v>39</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F45">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>25</v>
@@ -1399,27 +1404,27 @@
         <v>39</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F46">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F47">
         <v>1000</v>
@@ -1427,75 +1432,275 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D48" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="E48" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="E49" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F50">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F54">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F56">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1" t="s">
+      <c r="D60" s="1"/>
+      <c r="E60" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F50">
+      <c r="F60">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D56" s="1"/>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="1"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>